<commit_message>
Added edges from pathway-filtered metabolites
</commit_message>
<xml_diff>
--- a/project-2/data/processed/enrich_pathways_string.xlsx
+++ b/project-2/data/processed/enrich_pathways_string.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\MO413A\projeto\alternative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\MO413A\MO413-Ciencia-e-Visualizacao-de-Dados-em-Saude-2024\project-2\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D93D32C9-5E95-4C7D-9744-0E29BA3B3757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA8A365-BBA2-4FEB-8D44-0E6E1B44D0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{5DD13ED5-F404-4468-B56E-4DFFD5CBFC9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{5DD13ED5-F404-4468-B56E-4DFFD5CBFC9E}"/>
   </bookViews>
   <sheets>
     <sheet name="msea_ora_result" sheetId="2" r:id="rId1"/>
     <sheet name="differential_metabolites" sheetId="1" r:id="rId2"/>
-    <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha1" sheetId="4" r:id="rId3"/>
+    <sheet name="Planilha2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="551">
   <si>
     <t>Column1</t>
   </si>
@@ -773,13 +774,973 @@
   </si>
   <si>
     <t>https://www.kegg.jp/kegg-bin/show_pathway?hsa00020</t>
+  </si>
+  <si>
+    <t>C00011  </t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>C00014  </t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>C00025  </t>
+  </si>
+  <si>
+    <t>L-Glutamate</t>
+  </si>
+  <si>
+    <t>C00026  </t>
+  </si>
+  <si>
+    <t>2-Oxoglutarate</t>
+  </si>
+  <si>
+    <t>C00049  </t>
+  </si>
+  <si>
+    <t>L-Aspartate</t>
+  </si>
+  <si>
+    <t>C00062  </t>
+  </si>
+  <si>
+    <t>L-Arginine</t>
+  </si>
+  <si>
+    <t>C00064  </t>
+  </si>
+  <si>
+    <t>L-Glutamine</t>
+  </si>
+  <si>
+    <t>C00077  </t>
+  </si>
+  <si>
+    <t>L-Ornithine</t>
+  </si>
+  <si>
+    <t>C00086  </t>
+  </si>
+  <si>
+    <t>Urea</t>
+  </si>
+  <si>
+    <t>C00122  </t>
+  </si>
+  <si>
+    <t>Fumarate</t>
+  </si>
+  <si>
+    <t>C00169  </t>
+  </si>
+  <si>
+    <t>Carbamoyl phosphate</t>
+  </si>
+  <si>
+    <t>C00327  </t>
+  </si>
+  <si>
+    <t>L-Citrulline</t>
+  </si>
+  <si>
+    <t>C00437  </t>
+  </si>
+  <si>
+    <t>N-Acetylornithine</t>
+  </si>
+  <si>
+    <t>C00624  </t>
+  </si>
+  <si>
+    <t>N-Acetyl-L-glutamate</t>
+  </si>
+  <si>
+    <t>C01010  </t>
+  </si>
+  <si>
+    <t>Urea-1-carboxylate</t>
+  </si>
+  <si>
+    <t>C01250  </t>
+  </si>
+  <si>
+    <t>N-Acetyl-L-glutamate 5-semialdehyde</t>
+  </si>
+  <si>
+    <t>C03406  </t>
+  </si>
+  <si>
+    <t>N-(L-Arginino)succinate</t>
+  </si>
+  <si>
+    <t>C04133  </t>
+  </si>
+  <si>
+    <t>N-Acetyl-L-glutamate 5-phosphate</t>
+  </si>
+  <si>
+    <t>C15532  </t>
+  </si>
+  <si>
+    <t>N-Acetyl-L-citrulline</t>
+  </si>
+  <si>
+    <t>C20948  </t>
+  </si>
+  <si>
+    <t>LysW-L-glutamate</t>
+  </si>
+  <si>
+    <t>C20949  </t>
+  </si>
+  <si>
+    <t>LysW-L-glutamyl 5-phosphate</t>
+  </si>
+  <si>
+    <t>C20950  </t>
+  </si>
+  <si>
+    <t>LysW-L-glutamate 5-semialdehyde</t>
+  </si>
+  <si>
+    <t>C20951  </t>
+  </si>
+  <si>
+    <t>LysW-L-ornithine</t>
+  </si>
+  <si>
+    <t>C00022  </t>
+  </si>
+  <si>
+    <t>Pyruvate</t>
+  </si>
+  <si>
+    <t>C00024  </t>
+  </si>
+  <si>
+    <t>Acetyl-CoA</t>
+  </si>
+  <si>
+    <t>C00109  </t>
+  </si>
+  <si>
+    <t>2-Oxobutanoate</t>
+  </si>
+  <si>
+    <t>C00123  </t>
+  </si>
+  <si>
+    <t>L-Leucine</t>
+  </si>
+  <si>
+    <t>C00141  </t>
+  </si>
+  <si>
+    <t>3-Methyl-2-oxobutanoic acid</t>
+  </si>
+  <si>
+    <t>C00183  </t>
+  </si>
+  <si>
+    <t>L-Valine</t>
+  </si>
+  <si>
+    <t>C00188  </t>
+  </si>
+  <si>
+    <t>L-Threonine</t>
+  </si>
+  <si>
+    <t>C00233  </t>
+  </si>
+  <si>
+    <t>4-Methyl-2-oxopentanoate</t>
+  </si>
+  <si>
+    <t>C00407  </t>
+  </si>
+  <si>
+    <t>L-Isoleucine</t>
+  </si>
+  <si>
+    <t>C00671  </t>
+  </si>
+  <si>
+    <t>(S)-3-Methyl-2-oxopentanoic acid</t>
+  </si>
+  <si>
+    <t>C02226  </t>
+  </si>
+  <si>
+    <t>2-Methylmaleate</t>
+  </si>
+  <si>
+    <t>C02504  </t>
+  </si>
+  <si>
+    <t>alpha-Isopropylmalate</t>
+  </si>
+  <si>
+    <t>C02612  </t>
+  </si>
+  <si>
+    <t>(R)-2-Methylmalate</t>
+  </si>
+  <si>
+    <t>C02631  </t>
+  </si>
+  <si>
+    <t>2-Isopropylmaleate</t>
+  </si>
+  <si>
+    <t>C04181  </t>
+  </si>
+  <si>
+    <t>3-Hydroxy-3-methyl-2-oxobutanoic acid</t>
+  </si>
+  <si>
+    <t>C04236  </t>
+  </si>
+  <si>
+    <t>(2S)-2-Isopropyl-3-oxosuccinate</t>
+  </si>
+  <si>
+    <t>C04272  </t>
+  </si>
+  <si>
+    <t>(R)-2,3-Dihydroxy-3-methylbutanoate</t>
+  </si>
+  <si>
+    <t>C04411  </t>
+  </si>
+  <si>
+    <t>(2R,3S)-3-Isopropylmalate</t>
+  </si>
+  <si>
+    <t>C06006  </t>
+  </si>
+  <si>
+    <t>(S)-2-Aceto-2-hydroxybutanoate</t>
+  </si>
+  <si>
+    <t>C06007  </t>
+  </si>
+  <si>
+    <t>(R)-2,3-Dihydroxy-3-methylpentanoate</t>
+  </si>
+  <si>
+    <t>C06010  </t>
+  </si>
+  <si>
+    <t>(S)-2-Acetolactate</t>
+  </si>
+  <si>
+    <t>C06032  </t>
+  </si>
+  <si>
+    <t>D-erythro-3-Methylmalate</t>
+  </si>
+  <si>
+    <t>C14463  </t>
+  </si>
+  <si>
+    <t>(R)-3-Hydroxy-3-methyl-2-oxopentanoate</t>
+  </si>
+  <si>
+    <t>C00042  </t>
+  </si>
+  <si>
+    <t>Succinate</t>
+  </si>
+  <si>
+    <t>C00079  </t>
+  </si>
+  <si>
+    <t>L-Phenylalanine</t>
+  </si>
+  <si>
+    <t>C00082  </t>
+  </si>
+  <si>
+    <t>L-Tyrosine</t>
+  </si>
+  <si>
+    <t>C00084  </t>
+  </si>
+  <si>
+    <t>Acetaldehyde</t>
+  </si>
+  <si>
+    <t>C00091  </t>
+  </si>
+  <si>
+    <t>Succinyl-CoA</t>
+  </si>
+  <si>
+    <t>C00166  </t>
+  </si>
+  <si>
+    <t>Phenylpyruvate</t>
+  </si>
+  <si>
+    <t>C00423  </t>
+  </si>
+  <si>
+    <t>trans-Cinnamate</t>
+  </si>
+  <si>
+    <t>C00512  </t>
+  </si>
+  <si>
+    <t>Benzoyl-CoA</t>
+  </si>
+  <si>
+    <t>C00582  </t>
+  </si>
+  <si>
+    <t>Phenylacetyl-CoA</t>
+  </si>
+  <si>
+    <t>C00596  </t>
+  </si>
+  <si>
+    <t>2-Hydroxy-2,4-pentadienoate</t>
+  </si>
+  <si>
+    <t>C00601  </t>
+  </si>
+  <si>
+    <t>Phenylacetaldehyde</t>
+  </si>
+  <si>
+    <t>C00642  </t>
+  </si>
+  <si>
+    <t>4-Hydroxyphenylacetate</t>
+  </si>
+  <si>
+    <t>C01198  </t>
+  </si>
+  <si>
+    <t>3-(2-Hydroxyphenyl)propanoate</t>
+  </si>
+  <si>
+    <t>C01772  </t>
+  </si>
+  <si>
+    <t>trans-2-Hydroxycinnamate</t>
+  </si>
+  <si>
+    <t>C02137  </t>
+  </si>
+  <si>
+    <t>alpha-Oxo-benzeneacetic acid</t>
+  </si>
+  <si>
+    <t>C02232  </t>
+  </si>
+  <si>
+    <t>3-Oxoadipyl-CoA</t>
+  </si>
+  <si>
+    <t>C02265  </t>
+  </si>
+  <si>
+    <t>D-Phenylalanine</t>
+  </si>
+  <si>
+    <t>C02505  </t>
+  </si>
+  <si>
+    <t>2-Phenylacetamide</t>
+  </si>
+  <si>
+    <t>C02763  </t>
+  </si>
+  <si>
+    <t>2-Hydroxy-3-phenylpropenoate</t>
+  </si>
+  <si>
+    <t>C03519  </t>
+  </si>
+  <si>
+    <t>N-Acetyl-L-phenylalanine</t>
+  </si>
+  <si>
+    <t>C03589  </t>
+  </si>
+  <si>
+    <t>4-Hydroxy-2-oxopentanoate</t>
+  </si>
+  <si>
+    <t>C04044  </t>
+  </si>
+  <si>
+    <t>3-(2,3-Dihydroxyphenyl)propanoate</t>
+  </si>
+  <si>
+    <t>C04148  </t>
+  </si>
+  <si>
+    <t>Phenylacetylglutamine</t>
+  </si>
+  <si>
+    <t>C04479  </t>
+  </si>
+  <si>
+    <t>2-Hydroxy-6-oxonona-2,4-diene-1,9-dioate</t>
+  </si>
+  <si>
+    <t>C05332  </t>
+  </si>
+  <si>
+    <t>Phenethylamine</t>
+  </si>
+  <si>
+    <t>C05593  </t>
+  </si>
+  <si>
+    <t>3-Hydroxyphenylacetate</t>
+  </si>
+  <si>
+    <t>C05598  </t>
+  </si>
+  <si>
+    <t>Phenylacetylglycine</t>
+  </si>
+  <si>
+    <t>C05607  </t>
+  </si>
+  <si>
+    <t>Phenyllactate</t>
+  </si>
+  <si>
+    <t>C05629  </t>
+  </si>
+  <si>
+    <t>Phenylpropanoate</t>
+  </si>
+  <si>
+    <t>C05852  </t>
+  </si>
+  <si>
+    <t>2-Hydroxyphenylacetate</t>
+  </si>
+  <si>
+    <t>C05853  </t>
+  </si>
+  <si>
+    <t>Phenylethyl alcohol</t>
+  </si>
+  <si>
+    <t>C06207  </t>
+  </si>
+  <si>
+    <t>2,6-Dihydroxyphenylacetate</t>
+  </si>
+  <si>
+    <t>C07086  </t>
+  </si>
+  <si>
+    <t>Phenylacetic acid</t>
+  </si>
+  <si>
+    <t>C11457  </t>
+  </si>
+  <si>
+    <t>3-(3-Hydroxyphenyl)propanoic acid</t>
+  </si>
+  <si>
+    <t>C11588  </t>
+  </si>
+  <si>
+    <t>cis-3-(Carboxy-ethyl)-3,5-cyclo-hexadiene-1,2-diol</t>
+  </si>
+  <si>
+    <t>C12621  </t>
+  </si>
+  <si>
+    <t>trans-3-Hydroxycinnamate</t>
+  </si>
+  <si>
+    <t>C12622  </t>
+  </si>
+  <si>
+    <t>cis-3-(3-Carboxyethenyl)-3,5-cyclohexadiene-1,2-diol</t>
+  </si>
+  <si>
+    <t>C12623  </t>
+  </si>
+  <si>
+    <t>trans-2,3-Dihydroxycinnamate</t>
+  </si>
+  <si>
+    <t>C12624  </t>
+  </si>
+  <si>
+    <t>2-Hydroxy-6-ketononatrienedioate</t>
+  </si>
+  <si>
+    <t>C14144  </t>
+  </si>
+  <si>
+    <t>5-Carboxy-2-pentenoyl-CoA</t>
+  </si>
+  <si>
+    <t>C14145  </t>
+  </si>
+  <si>
+    <t>(3S)-3-Hydroxyadipyl-CoA</t>
+  </si>
+  <si>
+    <t>C15524  </t>
+  </si>
+  <si>
+    <t>Phenylglyoxylyl-CoA</t>
+  </si>
+  <si>
+    <t>C19945  </t>
+  </si>
+  <si>
+    <t>3-Oxo-5,6-dehydrosuberyl-CoA</t>
+  </si>
+  <si>
+    <t>C19946  </t>
+  </si>
+  <si>
+    <t>3-Oxo-5,6-dehydrosuberyl-CoA semialdehyde</t>
+  </si>
+  <si>
+    <t>C19975  </t>
+  </si>
+  <si>
+    <t>2-Oxepin-2(3H)-ylideneacetyl-CoA</t>
+  </si>
+  <si>
+    <t>C20062  </t>
+  </si>
+  <si>
+    <t>2-(1,2-Epoxy-1,2-dihydrophenyl)acetyl-CoA</t>
+  </si>
+  <si>
+    <t>C00005  </t>
+  </si>
+  <si>
+    <t>NADPH</t>
+  </si>
+  <si>
+    <t>C00006  </t>
+  </si>
+  <si>
+    <t>NADP+</t>
+  </si>
+  <si>
+    <t>C00037  </t>
+  </si>
+  <si>
+    <t>Glycine</t>
+  </si>
+  <si>
+    <t>C00051  </t>
+  </si>
+  <si>
+    <t>Glutathione</t>
+  </si>
+  <si>
+    <t>C00072  </t>
+  </si>
+  <si>
+    <t>Ascorbate</t>
+  </si>
+  <si>
+    <t>C00097  </t>
+  </si>
+  <si>
+    <t>L-Cysteine</t>
+  </si>
+  <si>
+    <t>C00127  </t>
+  </si>
+  <si>
+    <t>Glutathione disulfide</t>
+  </si>
+  <si>
+    <t>C00134  </t>
+  </si>
+  <si>
+    <t>Putrescine</t>
+  </si>
+  <si>
+    <t>C00151  </t>
+  </si>
+  <si>
+    <t>L-Amino acid</t>
+  </si>
+  <si>
+    <t>C00315  </t>
+  </si>
+  <si>
+    <t>Spermidine</t>
+  </si>
+  <si>
+    <t>C00669  </t>
+  </si>
+  <si>
+    <t>gamma-L-Glutamyl-L-cysteine</t>
+  </si>
+  <si>
+    <t>C00750  </t>
+  </si>
+  <si>
+    <t>Spermine</t>
+  </si>
+  <si>
+    <t>C01322  </t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>C01419  </t>
+  </si>
+  <si>
+    <t>Cys-Gly</t>
+  </si>
+  <si>
+    <t>C01672  </t>
+  </si>
+  <si>
+    <t>Cadaverine</t>
+  </si>
+  <si>
+    <t>C01879  </t>
+  </si>
+  <si>
+    <t>5-Oxoproline</t>
+  </si>
+  <si>
+    <t>C02090  </t>
+  </si>
+  <si>
+    <t>Trypanothione</t>
+  </si>
+  <si>
+    <t>C02320  </t>
+  </si>
+  <si>
+    <t>R-S-Glutathione</t>
+  </si>
+  <si>
+    <t>C03170  </t>
+  </si>
+  <si>
+    <t>Trypanothione disulfide</t>
+  </si>
+  <si>
+    <t>C03646  </t>
+  </si>
+  <si>
+    <t>Bis-gamma-glutamylcystine</t>
+  </si>
+  <si>
+    <t>C03740  </t>
+  </si>
+  <si>
+    <t>(5-L-Glutamyl)-L-amino acid</t>
+  </si>
+  <si>
+    <t>C05422  </t>
+  </si>
+  <si>
+    <t>Dehydroascorbate</t>
+  </si>
+  <si>
+    <t>C05726  </t>
+  </si>
+  <si>
+    <t>S-Substituted L-cysteine</t>
+  </si>
+  <si>
+    <t>C05727  </t>
+  </si>
+  <si>
+    <t>S-Substituted N-acetyl-L-cysteine</t>
+  </si>
+  <si>
+    <t>C05729  </t>
+  </si>
+  <si>
+    <t>R-S-Cysteinylglycine</t>
+  </si>
+  <si>
+    <t>C05730  </t>
+  </si>
+  <si>
+    <t>Glutathionylspermidine</t>
+  </si>
+  <si>
+    <t>C16562  </t>
+  </si>
+  <si>
+    <t>Glutathionylspermine</t>
+  </si>
+  <si>
+    <t>C16563  </t>
+  </si>
+  <si>
+    <t>Bis(glutathionyl)spermine</t>
+  </si>
+  <si>
+    <t>C16564  </t>
+  </si>
+  <si>
+    <t>Bis(glutathionyl)spermine disulfide</t>
+  </si>
+  <si>
+    <t>C16565  </t>
+  </si>
+  <si>
+    <t>Aminopropylcadaverine</t>
+  </si>
+  <si>
+    <t>C16566  </t>
+  </si>
+  <si>
+    <t>Glutathionylaminopropylcadaverine</t>
+  </si>
+  <si>
+    <t>C16567  </t>
+  </si>
+  <si>
+    <t>Homotrypanothione</t>
+  </si>
+  <si>
+    <t>C16568  </t>
+  </si>
+  <si>
+    <t>Homotrypanothione disulfide</t>
+  </si>
+  <si>
+    <t>C16663  </t>
+  </si>
+  <si>
+    <t>Tryparedoxin</t>
+  </si>
+  <si>
+    <t>C16664  </t>
+  </si>
+  <si>
+    <t>Tryparedoxin disulfide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Glutathione metabolism</t>
+  </si>
+  <si>
+    <t>C00074  </t>
+  </si>
+  <si>
+    <t>Phosphoenolpyruvate</t>
+  </si>
+  <si>
+    <t>C00078  </t>
+  </si>
+  <si>
+    <t>L-Tryptophan</t>
+  </si>
+  <si>
+    <t>C00108  </t>
+  </si>
+  <si>
+    <t>Anthranilate</t>
+  </si>
+  <si>
+    <t>C00119  </t>
+  </si>
+  <si>
+    <t>5-Phospho-alpha-D-ribose 1-diphosphate</t>
+  </si>
+  <si>
+    <t>C00230  </t>
+  </si>
+  <si>
+    <t>3,4-Dihydroxybenzoate</t>
+  </si>
+  <si>
+    <t>C00251  </t>
+  </si>
+  <si>
+    <t>Chorismate</t>
+  </si>
+  <si>
+    <t>C00254  </t>
+  </si>
+  <si>
+    <t>Prephenate</t>
+  </si>
+  <si>
+    <t>C00279  </t>
+  </si>
+  <si>
+    <t>D-Erythrose 4-phosphate</t>
+  </si>
+  <si>
+    <t>C00296  </t>
+  </si>
+  <si>
+    <t>Quinate</t>
+  </si>
+  <si>
+    <t>C00354  </t>
+  </si>
+  <si>
+    <t>D-Fructose 1,6-bisphosphate</t>
+  </si>
+  <si>
+    <t>C00441  </t>
+  </si>
+  <si>
+    <t>L-Aspartate 4-semialdehyde</t>
+  </si>
+  <si>
+    <t>C00463  </t>
+  </si>
+  <si>
+    <t>Indole</t>
+  </si>
+  <si>
+    <t>C00493  </t>
+  </si>
+  <si>
+    <t>Shikimate</t>
+  </si>
+  <si>
+    <t>C00587  </t>
+  </si>
+  <si>
+    <t>3-Hydroxybenzoate</t>
+  </si>
+  <si>
+    <t>C00826  </t>
+  </si>
+  <si>
+    <t>L-Arogenate</t>
+  </si>
+  <si>
+    <t>C00944  </t>
+  </si>
+  <si>
+    <t>3-Dehydroquinate</t>
+  </si>
+  <si>
+    <t>C01094  </t>
+  </si>
+  <si>
+    <t>D-Fructose 1-phosphate</t>
+  </si>
+  <si>
+    <t>C01179  </t>
+  </si>
+  <si>
+    <t>3-(4-Hydroxyphenyl)pyruvate</t>
+  </si>
+  <si>
+    <t>C01269  </t>
+  </si>
+  <si>
+    <t>5-O-(1-Carboxyvinyl)-3-phosphoshikimate</t>
+  </si>
+  <si>
+    <t>C01302  </t>
+  </si>
+  <si>
+    <t>1-(2-Carboxyphenylamino)-1-deoxy-D-ribulose 5-phosphate</t>
+  </si>
+  <si>
+    <t>C02637  </t>
+  </si>
+  <si>
+    <t>3-Dehydroshikimate</t>
+  </si>
+  <si>
+    <t>C03175  </t>
+  </si>
+  <si>
+    <t>Shikimate 3-phosphate</t>
+  </si>
+  <si>
+    <t>C03506  </t>
+  </si>
+  <si>
+    <t>Indoleglycerol phosphate</t>
+  </si>
+  <si>
+    <t>C04302  </t>
+  </si>
+  <si>
+    <t>N-(5-Phospho-D-ribosyl)anthranilate</t>
+  </si>
+  <si>
+    <t>C04691  </t>
+  </si>
+  <si>
+    <t>2-Dehydro-3-deoxy-D-arabino-heptonate 7-phosphate</t>
+  </si>
+  <si>
+    <t>C16848  </t>
+  </si>
+  <si>
+    <t>6-Deoxy-5-ketofructose 1-phosphate</t>
+  </si>
+  <si>
+    <t>C16850  </t>
+  </si>
+  <si>
+    <t>2-Amino-3,7-dideoxy-D-threo-hept-6-ulosonic acid</t>
+  </si>
+  <si>
+    <t>C17235  </t>
+  </si>
+  <si>
+    <t>L-Homophenylalanine</t>
+  </si>
+  <si>
+    <t>C20327  </t>
+  </si>
+  <si>
+    <t>2-Oxo-4-phenylbutyric acid</t>
+  </si>
+  <si>
+    <t>C20653  </t>
+  </si>
+  <si>
+    <t>2-Benzylmalic acid</t>
+  </si>
+  <si>
+    <t>C20654  </t>
+  </si>
+  <si>
+    <t>3-Benzylmalic acid</t>
+  </si>
+  <si>
+    <t>C20710  </t>
+  </si>
+  <si>
+    <t>(4R,5R)-4,5-Dihydroxycyclohexa-1(6),2-diene-1-carboxylate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Phenylalanine, tyrosine and tryptophan biosynthesis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -808,16 +1769,34 @@
       <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -825,14 +1804,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1312,8 +2377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC387EB7-3D2D-477B-B5B0-54883689F471}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD34" sqref="AD34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,8 +3722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438DBFE7-5FA2-44A1-846E-B07F1EC0C54D}">
   <dimension ref="A2:A134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J116" sqref="J116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3335,6 +4400,2044 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFC0384-17CA-41FD-9F39-A1BCC716FCF1}">
+  <dimension ref="A1:C168"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="C69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C96" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="C97" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C98" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C99" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C100" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="C101" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="C102" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C103" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="C104" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C105" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="C106" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C107" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="C108" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C109" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C110" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="C111" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="C112" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C113" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C114" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C115" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="C116" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C117" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C118" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C119" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C120" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C121" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="C122" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="C123" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="C124" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="C125" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C126" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="C127" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C128" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="C129" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C130" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C131" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="C132" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="C133" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="C134" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="C135" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C136" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C137" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="C138" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C139" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="C140" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="C141" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C142" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="C143" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="C144" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="C145" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="C146" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="C147" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="C148" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C149" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="C150" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="C151" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="C152" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="C153" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="C154" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="C155" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="C156" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="C157" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="C158" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="C159" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="C160" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C161" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="C162" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C163" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="C164" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="C165" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="C166" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="C167" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="C168" t="s">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.genome.jp/entry/C00011" xr:uid="{8822741F-5F9F-4598-8E19-7BC79BDFF6B1}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://www.genome.jp/entry/C00014" xr:uid="{6E3B5764-5094-4802-B716-A797DAF54289}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://www.genome.jp/entry/C00025" xr:uid="{5C7A26E4-78B1-449F-AA06-26A3144373E2}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://www.genome.jp/entry/C00026" xr:uid="{43966885-4656-4E4E-881C-550C88852E87}"/>
+    <hyperlink ref="A5" r:id="rId5" display="https://www.genome.jp/entry/C00049" xr:uid="{84CEBCA3-1625-40C1-B32C-A5A9AAF0CE7E}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://www.genome.jp/entry/C00062" xr:uid="{E3AB85AE-C836-4781-9005-E909866930F0}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://www.genome.jp/entry/C00064" xr:uid="{BC4E04C2-81D7-4139-B241-7A03240EE27C}"/>
+    <hyperlink ref="A8" r:id="rId8" display="https://www.genome.jp/entry/C00077" xr:uid="{214C7113-7751-4032-9924-8EB8DCC2B45F}"/>
+    <hyperlink ref="A9" r:id="rId9" display="https://www.genome.jp/entry/C00086" xr:uid="{034F722D-FC27-43FE-B48E-FD6C371A0D3C}"/>
+    <hyperlink ref="A10" r:id="rId10" display="https://www.genome.jp/entry/C00122" xr:uid="{2AEF83FA-AC92-4636-ACB2-5EF3E01E0881}"/>
+    <hyperlink ref="A11" r:id="rId11" display="https://www.genome.jp/entry/C00169" xr:uid="{3D93CBDC-8A73-4A15-9291-DE0F1601F689}"/>
+    <hyperlink ref="A12" r:id="rId12" display="https://www.genome.jp/entry/C00327" xr:uid="{20CA5A2B-BEA5-4A01-BCB0-93361A0BF111}"/>
+    <hyperlink ref="A13" r:id="rId13" display="https://www.genome.jp/entry/C00437" xr:uid="{5E84425E-EF0B-4327-B055-A714DEE56DC7}"/>
+    <hyperlink ref="A14" r:id="rId14" display="https://www.genome.jp/entry/C00624" xr:uid="{E67D6D2D-357F-4A3B-A914-5442EC9C53A0}"/>
+    <hyperlink ref="A15" r:id="rId15" display="https://www.genome.jp/entry/C01010" xr:uid="{E15FC95E-F196-4782-B02A-66A7FB808ECB}"/>
+    <hyperlink ref="A16" r:id="rId16" display="https://www.genome.jp/entry/C01250" xr:uid="{57A47181-8C78-4B36-AE9C-4712A0D2243E}"/>
+    <hyperlink ref="A17" r:id="rId17" display="https://www.genome.jp/entry/C03406" xr:uid="{EE63A0F3-6F28-49E0-B6D9-4B4DCD400EBF}"/>
+    <hyperlink ref="A18" r:id="rId18" display="https://www.genome.jp/entry/C04133" xr:uid="{A2DF16C7-67CB-4716-8F52-0FF9BE4ACD55}"/>
+    <hyperlink ref="A19" r:id="rId19" display="https://www.genome.jp/entry/C15532" xr:uid="{804A2256-E158-4AC3-8A03-CA5707AE68E5}"/>
+    <hyperlink ref="A20" r:id="rId20" display="https://www.genome.jp/entry/C20948" xr:uid="{4547D5F3-02C4-448B-80F3-E2639CA921FC}"/>
+    <hyperlink ref="A21" r:id="rId21" display="https://www.genome.jp/entry/C20949" xr:uid="{5E3490EE-C821-478C-8455-1F1FAC6464E3}"/>
+    <hyperlink ref="A22" r:id="rId22" display="https://www.genome.jp/entry/C20950" xr:uid="{3DB17617-CA03-48F0-AA74-8D330D87E568}"/>
+    <hyperlink ref="A23" r:id="rId23" display="https://www.genome.jp/entry/C20951" xr:uid="{BF2DF59C-BA26-4437-846D-0D555832CDD8}"/>
+    <hyperlink ref="A24" r:id="rId24" display="https://www.kegg.jp/entry/C00022" xr:uid="{3DD3CBED-3982-4623-AEE8-EE7D7EC532EF}"/>
+    <hyperlink ref="A25" r:id="rId25" display="https://www.kegg.jp/entry/C00024" xr:uid="{5A222C5E-6E46-4590-99C6-F3F11A079ABE}"/>
+    <hyperlink ref="A26" r:id="rId26" display="https://www.kegg.jp/entry/C00109" xr:uid="{50260467-364D-4D4F-81A7-65176303CDDC}"/>
+    <hyperlink ref="A27" r:id="rId27" display="https://www.kegg.jp/entry/C00123" xr:uid="{3B102C9D-6071-45B3-83AF-5FA19FA16976}"/>
+    <hyperlink ref="A28" r:id="rId28" display="https://www.kegg.jp/entry/C00141" xr:uid="{9DDFB330-821E-4668-A91B-8D48AE1DB485}"/>
+    <hyperlink ref="A29" r:id="rId29" display="https://www.kegg.jp/entry/C00183" xr:uid="{BE78086F-0F5E-49FF-890F-CF4589F5FF79}"/>
+    <hyperlink ref="A30" r:id="rId30" display="https://www.kegg.jp/entry/C00188" xr:uid="{9AEFC6CA-FAD6-4709-B0F2-2FC932679EE4}"/>
+    <hyperlink ref="A31" r:id="rId31" display="https://www.kegg.jp/entry/C00233" xr:uid="{1E6205AF-BD20-4CDA-8985-5414AA644270}"/>
+    <hyperlink ref="A32" r:id="rId32" display="https://www.kegg.jp/entry/C00407" xr:uid="{E7B233D2-F255-420F-BA48-840B999A9822}"/>
+    <hyperlink ref="A33" r:id="rId33" display="https://www.kegg.jp/entry/C00671" xr:uid="{4DCE7BDF-0E97-47ED-BF24-255A9FACA166}"/>
+    <hyperlink ref="A34" r:id="rId34" display="https://www.kegg.jp/entry/C02226" xr:uid="{03FC5FC0-D3AD-4EE2-901C-FD8E7796C49E}"/>
+    <hyperlink ref="A35" r:id="rId35" display="https://www.kegg.jp/entry/C02504" xr:uid="{5646169A-411F-4F95-A2FC-E96FFE073033}"/>
+    <hyperlink ref="A36" r:id="rId36" display="https://www.kegg.jp/entry/C02612" xr:uid="{AD12BDAE-A273-46C9-980A-7373EF155BD2}"/>
+    <hyperlink ref="A37" r:id="rId37" display="https://www.kegg.jp/entry/C02631" xr:uid="{A409CC9A-BFAC-463C-90BE-F9262A83B55B}"/>
+    <hyperlink ref="A38" r:id="rId38" display="https://www.kegg.jp/entry/C04181" xr:uid="{92764FCC-388D-4D37-B0E2-907DD17A2403}"/>
+    <hyperlink ref="A39" r:id="rId39" display="https://www.kegg.jp/entry/C04236" xr:uid="{2F1FEE32-6F45-41C0-B787-27601721599B}"/>
+    <hyperlink ref="A40" r:id="rId40" display="https://www.kegg.jp/entry/C04272" xr:uid="{253620E2-BF05-47FC-A432-BE746FF172AC}"/>
+    <hyperlink ref="A41" r:id="rId41" display="https://www.kegg.jp/entry/C04411" xr:uid="{A3782C36-7FE0-4A89-A8CE-41D02EC40E7C}"/>
+    <hyperlink ref="A42" r:id="rId42" display="https://www.kegg.jp/entry/C06006" xr:uid="{DE984484-81AE-4CA8-8337-FB20359E60B3}"/>
+    <hyperlink ref="A43" r:id="rId43" display="https://www.kegg.jp/entry/C06007" xr:uid="{7BC7DCC5-D1D8-40CD-ADE4-58AF62B33537}"/>
+    <hyperlink ref="A44" r:id="rId44" display="https://www.kegg.jp/entry/C06010" xr:uid="{F3DFB7AF-8DB5-4B66-8C12-135888A8D005}"/>
+    <hyperlink ref="A45" r:id="rId45" display="https://www.kegg.jp/entry/C06032" xr:uid="{6A1711E2-091F-4981-A5D6-5A456612A2A6}"/>
+    <hyperlink ref="A46" r:id="rId46" display="https://www.kegg.jp/entry/C14463" xr:uid="{19C1B6AC-E847-40A6-8C7C-0B3D114F52ED}"/>
+    <hyperlink ref="A47" r:id="rId47" display="https://www.kegg.jp/entry/C00022" xr:uid="{C6003F8F-2BF8-490A-8967-439482F7AA1F}"/>
+    <hyperlink ref="A48" r:id="rId48" display="https://www.kegg.jp/entry/C00024" xr:uid="{6D8039B7-0BE5-4F02-8877-77091B5868A1}"/>
+    <hyperlink ref="A49" r:id="rId49" display="https://www.kegg.jp/entry/C00042" xr:uid="{1199672D-9A65-4B46-AC7B-396441A189F3}"/>
+    <hyperlink ref="A50" r:id="rId50" display="https://www.kegg.jp/entry/C00079" xr:uid="{94E7BF8E-69AB-4D22-8693-326207174160}"/>
+    <hyperlink ref="A51" r:id="rId51" display="https://www.kegg.jp/entry/C00082" xr:uid="{EBE1F36A-F100-47B5-9899-7D7BCC1BCBF9}"/>
+    <hyperlink ref="A52" r:id="rId52" display="https://www.kegg.jp/entry/C00084" xr:uid="{59F4BA7A-2A0C-488F-B4A4-1F9B6E69BD60}"/>
+    <hyperlink ref="A53" r:id="rId53" display="https://www.kegg.jp/entry/C00091" xr:uid="{FFEBF5FC-1911-410F-B80C-6C01FB157FCF}"/>
+    <hyperlink ref="A54" r:id="rId54" display="https://www.kegg.jp/entry/C00122" xr:uid="{52D71B32-F502-41B5-8C04-32678A9B49D2}"/>
+    <hyperlink ref="A55" r:id="rId55" display="https://www.kegg.jp/entry/C00166" xr:uid="{8EDA76A6-98A9-4417-A8F5-F729A4E3531E}"/>
+    <hyperlink ref="A56" r:id="rId56" display="https://www.kegg.jp/entry/C00423" xr:uid="{D62466BD-C0A0-43FC-BBC9-3FF623EFBE9D}"/>
+    <hyperlink ref="A57" r:id="rId57" display="https://www.kegg.jp/entry/C00512" xr:uid="{6E9A4953-32E3-404D-B03D-2FA79A9D77EA}"/>
+    <hyperlink ref="A58" r:id="rId58" display="https://www.kegg.jp/entry/C00582" xr:uid="{B4FC02CF-F330-4B94-9CC3-310842CD8FBB}"/>
+    <hyperlink ref="A59" r:id="rId59" display="https://www.kegg.jp/entry/C00596" xr:uid="{3441DD20-C54E-4045-834D-12203DB02F25}"/>
+    <hyperlink ref="A60" r:id="rId60" display="https://www.kegg.jp/entry/C00601" xr:uid="{17E01EB5-F4DB-4CF9-9EC3-502C768E8F03}"/>
+    <hyperlink ref="A61" r:id="rId61" display="https://www.kegg.jp/entry/C00642" xr:uid="{A6CC3AA7-284D-49C4-B894-CA6C65D447C7}"/>
+    <hyperlink ref="A62" r:id="rId62" display="https://www.kegg.jp/entry/C01198" xr:uid="{08401305-A0F9-4769-860D-00509CCFC960}"/>
+    <hyperlink ref="A63" r:id="rId63" display="https://www.kegg.jp/entry/C01772" xr:uid="{C1F8645D-8EE2-4092-AADC-F559D9E012F4}"/>
+    <hyperlink ref="A64" r:id="rId64" display="https://www.kegg.jp/entry/C02137" xr:uid="{02FFF4E5-E5E6-4147-B4B1-D824176B14E4}"/>
+    <hyperlink ref="A65" r:id="rId65" display="https://www.kegg.jp/entry/C02232" xr:uid="{8C0CE321-9A6A-47F3-BB06-70F1AED1AFB5}"/>
+    <hyperlink ref="A66" r:id="rId66" display="https://www.kegg.jp/entry/C02265" xr:uid="{24D27028-598A-4A17-8ECA-3B8FBBFFBE2E}"/>
+    <hyperlink ref="A67" r:id="rId67" display="https://www.kegg.jp/entry/C02505" xr:uid="{3ADE7A5B-2247-4FFD-906D-A5105182838B}"/>
+    <hyperlink ref="A68" r:id="rId68" display="https://www.kegg.jp/entry/C02763" xr:uid="{CF34CC4E-EA29-4AE1-A3B0-0D66B5E5424D}"/>
+    <hyperlink ref="A69" r:id="rId69" display="https://www.kegg.jp/entry/C03519" xr:uid="{A96FE20C-246B-4380-8108-BC32EE56241E}"/>
+    <hyperlink ref="A70" r:id="rId70" display="https://www.kegg.jp/entry/C03589" xr:uid="{D84C3335-A6E1-43C8-8D0C-427F091EBF91}"/>
+    <hyperlink ref="A71" r:id="rId71" display="https://www.kegg.jp/entry/C04044" xr:uid="{EEB5A5CA-B2EE-4BDB-92FE-AAC6CAECD75C}"/>
+    <hyperlink ref="A72" r:id="rId72" display="https://www.kegg.jp/entry/C04148" xr:uid="{473A18FD-27D5-463D-BAC6-29BF2792C6C4}"/>
+    <hyperlink ref="A73" r:id="rId73" display="https://www.kegg.jp/entry/C04479" xr:uid="{F8DB50DA-3022-4646-9EEC-95A2CDA2C452}"/>
+    <hyperlink ref="A74" r:id="rId74" display="https://www.kegg.jp/entry/C05332" xr:uid="{05FE6FA4-3472-41BC-B08C-6261EA7ADA09}"/>
+    <hyperlink ref="A75" r:id="rId75" display="https://www.kegg.jp/entry/C05593" xr:uid="{ABE9CD27-462D-43DF-9BC8-9008C00864B8}"/>
+    <hyperlink ref="A76" r:id="rId76" display="https://www.kegg.jp/entry/C05598" xr:uid="{B1A62E64-E4D2-45B6-9A9A-4C7A770F03E1}"/>
+    <hyperlink ref="A77" r:id="rId77" display="https://www.kegg.jp/entry/C05607" xr:uid="{8DF12265-0A3E-45F9-BC3A-FBA1A122D429}"/>
+    <hyperlink ref="A78" r:id="rId78" display="https://www.kegg.jp/entry/C05629" xr:uid="{98246768-60A9-46B7-9CA4-CEDBF00E2DB3}"/>
+    <hyperlink ref="A79" r:id="rId79" display="https://www.kegg.jp/entry/C05852" xr:uid="{E26E9BD7-C94D-42BA-A879-D3C6C27CE2E1}"/>
+    <hyperlink ref="A80" r:id="rId80" display="https://www.kegg.jp/entry/C05853" xr:uid="{56BB9087-C8E9-4561-B287-84C95F7FD674}"/>
+    <hyperlink ref="A81" r:id="rId81" display="https://www.kegg.jp/entry/C06207" xr:uid="{2D4E23FB-B774-4B96-A582-9F8F25503458}"/>
+    <hyperlink ref="A82" r:id="rId82" display="https://www.kegg.jp/entry/C07086" xr:uid="{A18C3A30-0359-423A-9320-8C8CC136BF16}"/>
+    <hyperlink ref="A83" r:id="rId83" display="https://www.kegg.jp/entry/C11457" xr:uid="{5E4F0678-F5AD-4A6A-AF57-B1259C4543A4}"/>
+    <hyperlink ref="A84" r:id="rId84" display="https://www.kegg.jp/entry/C11588" xr:uid="{C60A6795-6110-426D-809A-3A09B1F829FC}"/>
+    <hyperlink ref="A85" r:id="rId85" display="https://www.kegg.jp/entry/C12621" xr:uid="{72A1DE83-FC7D-4FAD-B6EA-143185606972}"/>
+    <hyperlink ref="A86" r:id="rId86" display="https://www.kegg.jp/entry/C12622" xr:uid="{857697DC-5C72-4375-AA29-35B761246431}"/>
+    <hyperlink ref="A87" r:id="rId87" display="https://www.kegg.jp/entry/C12623" xr:uid="{8D34591A-B47E-4544-AE99-6749CB708CFE}"/>
+    <hyperlink ref="A88" r:id="rId88" display="https://www.kegg.jp/entry/C12624" xr:uid="{50CF3C3D-AFB8-415E-B557-7C9E66F939F7}"/>
+    <hyperlink ref="A89" r:id="rId89" display="https://www.kegg.jp/entry/C14144" xr:uid="{32B07D2A-4196-4AC2-89E8-292E843DF88D}"/>
+    <hyperlink ref="A90" r:id="rId90" display="https://www.kegg.jp/entry/C14145" xr:uid="{F2B79D95-528E-43AC-A078-91ED35034E82}"/>
+    <hyperlink ref="A91" r:id="rId91" display="https://www.kegg.jp/entry/C15524" xr:uid="{E138FCB2-B032-4071-B88D-EA0B52941EC1}"/>
+    <hyperlink ref="A92" r:id="rId92" display="https://www.kegg.jp/entry/C19945" xr:uid="{5BA392A2-BB4A-4D2B-8E04-4A948EB9BA89}"/>
+    <hyperlink ref="A93" r:id="rId93" display="https://www.kegg.jp/entry/C19946" xr:uid="{C0DD0943-25A2-4F43-A6F5-FF833A1825B5}"/>
+    <hyperlink ref="A94" r:id="rId94" display="https://www.kegg.jp/entry/C19975" xr:uid="{A9495FF6-66C7-4D7D-B51D-48C49C1DCFA6}"/>
+    <hyperlink ref="A95" r:id="rId95" display="https://www.kegg.jp/entry/C20062" xr:uid="{0B9514A5-4E01-474C-80E8-C8E82D9AD40C}"/>
+    <hyperlink ref="A96" r:id="rId96" display="https://www.kegg.jp/entry/C00005" xr:uid="{5FA53AEC-DDE6-4B5E-BA1B-E2E20FF2DAA9}"/>
+    <hyperlink ref="A97" r:id="rId97" display="https://www.kegg.jp/entry/C00006" xr:uid="{C16483D6-BAEB-4BEA-AE59-26AA78FEC79F}"/>
+    <hyperlink ref="A98" r:id="rId98" display="https://www.kegg.jp/entry/C00024" xr:uid="{1E8C9F23-E1F5-453F-BE6C-DB5750CA21B9}"/>
+    <hyperlink ref="A99" r:id="rId99" display="https://www.kegg.jp/entry/C00025" xr:uid="{06F5162B-65E4-46AE-B304-87722EC60C88}"/>
+    <hyperlink ref="A100" r:id="rId100" display="https://www.kegg.jp/entry/C00037" xr:uid="{74ADF40A-7610-4BA2-8F68-268EC2DC8336}"/>
+    <hyperlink ref="A101" r:id="rId101" display="https://www.kegg.jp/entry/C00051" xr:uid="{45DBCE53-E22C-47C2-8EAB-74BE40FE216E}"/>
+    <hyperlink ref="A102" r:id="rId102" display="https://www.kegg.jp/entry/C00072" xr:uid="{B92DACC0-EC16-4607-9F4F-74BE8678589D}"/>
+    <hyperlink ref="A103" r:id="rId103" display="https://www.kegg.jp/entry/C00077" xr:uid="{8FB60D0C-D553-4C09-9944-799FBA4DB41C}"/>
+    <hyperlink ref="A104" r:id="rId104" display="https://www.kegg.jp/entry/C00097" xr:uid="{7889E5E2-4EB1-45F1-83DE-7E300A8846DA}"/>
+    <hyperlink ref="A105" r:id="rId105" display="https://www.kegg.jp/entry/C00127" xr:uid="{2BBEADBA-58C4-4324-A56B-167D72B58308}"/>
+    <hyperlink ref="A106" r:id="rId106" display="https://www.kegg.jp/entry/C00134" xr:uid="{4880B355-BBC6-45C0-BD39-0BC18FC485E2}"/>
+    <hyperlink ref="A107" r:id="rId107" display="https://www.kegg.jp/entry/C00151" xr:uid="{307B9256-EC4B-4198-B65C-67965B1952A4}"/>
+    <hyperlink ref="A108" r:id="rId108" display="https://www.kegg.jp/entry/C00315" xr:uid="{9B16808C-FD57-4126-B604-48FC1499544B}"/>
+    <hyperlink ref="A109" r:id="rId109" display="https://www.kegg.jp/entry/C00669" xr:uid="{D635A9A9-CB04-45F3-88B5-5572D0E2C134}"/>
+    <hyperlink ref="A110" r:id="rId110" display="https://www.kegg.jp/entry/C00750" xr:uid="{7F4ECFE0-486B-4AE0-948D-B6462471250F}"/>
+    <hyperlink ref="A111" r:id="rId111" display="https://www.kegg.jp/entry/C01322" xr:uid="{82A21578-7C0A-4922-85C6-ABA95D6D3921}"/>
+    <hyperlink ref="A112" r:id="rId112" display="https://www.kegg.jp/entry/C01419" xr:uid="{1FE1CC7D-DF8A-43B2-9A24-B013BC2E7C3F}"/>
+    <hyperlink ref="A113" r:id="rId113" display="https://www.kegg.jp/entry/C01672" xr:uid="{90AA9B88-47BC-45F9-B7E0-978E75C6B923}"/>
+    <hyperlink ref="A114" r:id="rId114" display="https://www.kegg.jp/entry/C01879" xr:uid="{93E3E1F5-9B6F-4B20-AB6C-EAF2FF3077B0}"/>
+    <hyperlink ref="A115" r:id="rId115" display="https://www.kegg.jp/entry/C02090" xr:uid="{C4C98370-C578-49AA-B840-4FEB6A2914BC}"/>
+    <hyperlink ref="A116" r:id="rId116" display="https://www.kegg.jp/entry/C02320" xr:uid="{596901E6-2E7C-40D4-8CB2-229D5355BC2E}"/>
+    <hyperlink ref="A117" r:id="rId117" display="https://www.kegg.jp/entry/C03170" xr:uid="{EF65A5BD-B4C5-45E6-9970-5731AF088BF8}"/>
+    <hyperlink ref="A118" r:id="rId118" display="https://www.kegg.jp/entry/C03646" xr:uid="{04A86E0C-2776-4C7D-8D56-3B3A143B4CFE}"/>
+    <hyperlink ref="A119" r:id="rId119" display="https://www.kegg.jp/entry/C03740" xr:uid="{721F69F6-5996-4FC5-BE48-4F6CA6E5641E}"/>
+    <hyperlink ref="A120" r:id="rId120" display="https://www.kegg.jp/entry/C05422" xr:uid="{A5AE463A-BA24-4FF5-AE09-E29B0859E98D}"/>
+    <hyperlink ref="A121" r:id="rId121" display="https://www.kegg.jp/entry/C05726" xr:uid="{B4215DC6-0EE4-409F-BB31-4D8EA8A06955}"/>
+    <hyperlink ref="A122" r:id="rId122" display="https://www.kegg.jp/entry/C05727" xr:uid="{0045414D-5151-4C7F-BA3E-582B9904AFB8}"/>
+    <hyperlink ref="A123" r:id="rId123" display="https://www.kegg.jp/entry/C05729" xr:uid="{51D081AF-7328-43E8-92F2-54EC1EBB069D}"/>
+    <hyperlink ref="A124" r:id="rId124" display="https://www.kegg.jp/entry/C05730" xr:uid="{DFEED9A1-B8E9-41FB-8A93-0AC973B49CC7}"/>
+    <hyperlink ref="A125" r:id="rId125" display="https://www.kegg.jp/entry/C16562" xr:uid="{0303FE87-AA31-4BFD-9621-CDC1A0FF7C49}"/>
+    <hyperlink ref="A126" r:id="rId126" display="https://www.kegg.jp/entry/C16563" xr:uid="{538952AA-06A6-4327-9D27-DF688D1EC6FE}"/>
+    <hyperlink ref="A127" r:id="rId127" display="https://www.kegg.jp/entry/C16564" xr:uid="{3346FB91-3326-43EA-A2E9-518DD89750E2}"/>
+    <hyperlink ref="A128" r:id="rId128" display="https://www.kegg.jp/entry/C16565" xr:uid="{BAAA13C8-D82D-4600-AA79-C893E33383A1}"/>
+    <hyperlink ref="A129" r:id="rId129" display="https://www.kegg.jp/entry/C16566" xr:uid="{5A596889-87A3-47C2-8736-3BB6DBB1743B}"/>
+    <hyperlink ref="A130" r:id="rId130" display="https://www.kegg.jp/entry/C16567" xr:uid="{51541ABD-F204-4EE8-A851-1B72C0CFBD38}"/>
+    <hyperlink ref="A131" r:id="rId131" display="https://www.kegg.jp/entry/C16568" xr:uid="{550670FB-A27F-4453-A9AA-53729B68B27A}"/>
+    <hyperlink ref="A132" r:id="rId132" display="https://www.kegg.jp/entry/C16663" xr:uid="{B52E3706-9016-47E3-A526-F8D7DD06E72B}"/>
+    <hyperlink ref="A133" r:id="rId133" display="https://www.kegg.jp/entry/C16664" xr:uid="{E901875B-9CBD-463F-A7F4-94F4A0480F75}"/>
+    <hyperlink ref="A134" r:id="rId134" display="https://www.kegg.jp/entry/C00074" xr:uid="{F8EEB616-1141-4B21-8681-02EA6EF8AB81}"/>
+    <hyperlink ref="A135" r:id="rId135" display="https://www.kegg.jp/entry/C00078" xr:uid="{21AFC029-CB81-4876-8BAB-9C75CDD040BB}"/>
+    <hyperlink ref="A136" r:id="rId136" display="https://www.kegg.jp/entry/C00079" xr:uid="{56515F93-F1C6-40AC-8E5E-69D5CC0B2AA4}"/>
+    <hyperlink ref="A137" r:id="rId137" display="https://www.kegg.jp/entry/C00082" xr:uid="{A53345BB-4315-44AE-B95A-3CB8120D1C4A}"/>
+    <hyperlink ref="A138" r:id="rId138" display="https://www.kegg.jp/entry/C00108" xr:uid="{CC2F8BBF-6807-4266-A38E-F5DC94E677FE}"/>
+    <hyperlink ref="A139" r:id="rId139" display="https://www.kegg.jp/entry/C00119" xr:uid="{8C27ADF6-3400-4F53-8C41-8C1A2B77B4AA}"/>
+    <hyperlink ref="A140" r:id="rId140" display="https://www.kegg.jp/entry/C00166" xr:uid="{03FCB98F-0D26-467C-8CAA-2470E528C7C3}"/>
+    <hyperlink ref="A141" r:id="rId141" display="https://www.kegg.jp/entry/C00230" xr:uid="{7AEEC7C7-7609-4582-8409-CBC2DB7E002C}"/>
+    <hyperlink ref="A142" r:id="rId142" display="https://www.kegg.jp/entry/C00251" xr:uid="{54C26274-C89B-4E85-BC55-542CDEFD0C18}"/>
+    <hyperlink ref="A143" r:id="rId143" display="https://www.kegg.jp/entry/C00254" xr:uid="{D7D5C608-C15F-494D-8368-438CC47C3247}"/>
+    <hyperlink ref="A144" r:id="rId144" display="https://www.kegg.jp/entry/C00279" xr:uid="{F04711B1-B6F8-4F15-AA7F-FB4740AC5C53}"/>
+    <hyperlink ref="A145" r:id="rId145" display="https://www.kegg.jp/entry/C00296" xr:uid="{FA434DC0-DA1C-488F-921E-4D5393971FF3}"/>
+    <hyperlink ref="A146" r:id="rId146" display="https://www.kegg.jp/entry/C00354" xr:uid="{E5A22284-7079-4C6D-B755-5DCDE816191D}"/>
+    <hyperlink ref="A147" r:id="rId147" display="https://www.kegg.jp/entry/C00441" xr:uid="{5FBFB7E8-A101-49F0-AD45-A50463707A4D}"/>
+    <hyperlink ref="A148" r:id="rId148" display="https://www.kegg.jp/entry/C00463" xr:uid="{FD4C7D66-7A22-426E-B9EE-14B6C6847B24}"/>
+    <hyperlink ref="A149" r:id="rId149" display="https://www.kegg.jp/entry/C00493" xr:uid="{4CC95417-88FF-43D9-B829-F51D441757C5}"/>
+    <hyperlink ref="A150" r:id="rId150" display="https://www.kegg.jp/entry/C00587" xr:uid="{8C77ACE9-FC53-450A-8897-FD2902E98A6A}"/>
+    <hyperlink ref="A151" r:id="rId151" display="https://www.kegg.jp/entry/C00826" xr:uid="{78D3AEF3-07E7-448B-B7AC-2034BD865373}"/>
+    <hyperlink ref="A152" r:id="rId152" display="https://www.kegg.jp/entry/C00944" xr:uid="{BCB7B3EC-2D8C-4BDC-94B5-29FCB531515B}"/>
+    <hyperlink ref="A153" r:id="rId153" display="https://www.kegg.jp/entry/C01094" xr:uid="{09DF4066-3B18-47E5-914A-1F960A73A949}"/>
+    <hyperlink ref="A154" r:id="rId154" display="https://www.kegg.jp/entry/C01179" xr:uid="{4E845861-A2B9-47F9-9804-EA12ED19526F}"/>
+    <hyperlink ref="A155" r:id="rId155" display="https://www.kegg.jp/entry/C01269" xr:uid="{E18A3012-001C-446E-8B92-682F16B3F59A}"/>
+    <hyperlink ref="A156" r:id="rId156" display="https://www.kegg.jp/entry/C01302" xr:uid="{069A5375-C24E-43A2-80C8-F97C2B73FDD0}"/>
+    <hyperlink ref="A157" r:id="rId157" display="https://www.kegg.jp/entry/C02637" xr:uid="{CD6C7C75-E98C-4026-89DC-FF8F4DA0B7C1}"/>
+    <hyperlink ref="A158" r:id="rId158" display="https://www.kegg.jp/entry/C03175" xr:uid="{BDB2A6A8-A5CA-4345-A303-A766953A8137}"/>
+    <hyperlink ref="A159" r:id="rId159" display="https://www.kegg.jp/entry/C03506" xr:uid="{28FADC96-8CE3-44EC-8744-401DE07F22E0}"/>
+    <hyperlink ref="A160" r:id="rId160" display="https://www.kegg.jp/entry/C04302" xr:uid="{224966F6-19AB-45F8-93EB-1F6AFF395B93}"/>
+    <hyperlink ref="A161" r:id="rId161" display="https://www.kegg.jp/entry/C04691" xr:uid="{91B27DB9-0A58-459F-B3BE-4DD9C9872457}"/>
+    <hyperlink ref="A162" r:id="rId162" display="https://www.kegg.jp/entry/C16848" xr:uid="{48DD6098-E384-4271-B538-091B71A8D8F9}"/>
+    <hyperlink ref="A163" r:id="rId163" display="https://www.kegg.jp/entry/C16850" xr:uid="{BC326697-4491-49EE-A0F4-F72FB7936534}"/>
+    <hyperlink ref="A164" r:id="rId164" display="https://www.kegg.jp/entry/C17235" xr:uid="{DE523DCA-2F7C-47C1-8D55-480EA2EE9528}"/>
+    <hyperlink ref="A165" r:id="rId165" display="https://www.kegg.jp/entry/C20327" xr:uid="{F21359C0-A0C3-4BFE-B264-D22F20369FBC}"/>
+    <hyperlink ref="A166" r:id="rId166" display="https://www.kegg.jp/entry/C20653" xr:uid="{926840A8-67A5-4A38-869B-98C3F2997502}"/>
+    <hyperlink ref="A167" r:id="rId167" display="https://www.kegg.jp/entry/C20654" xr:uid="{7925FC6E-8D27-40FC-AA89-AB6EFE214F04}"/>
+    <hyperlink ref="A168" r:id="rId168" display="https://www.kegg.jp/entry/C20710" xr:uid="{8DA143BF-5F88-4E46-9DBA-E4A0A677E204}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92142D36-7CE9-4E9E-B4FF-775FCF3D35F0}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>